<commit_message>
Uploading single feature layers for all (1) zoned and (2) unzoned jurisdictions analyzed to date.
</commit_message>
<xml_diff>
--- a/ZoningAtlas/raw_data/Excel_workbooks/Essex_Concord_Features.xlsx
+++ b/ZoningAtlas/raw_data/Excel_workbooks/Essex_Concord_Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ybird/ZoningAtlas/VT_Zoning_Atlas/ZoningAtlas/raw_data/Excel_workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE86E08-F0DE-2645-9B6F-B046AB0D0F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A9B52F-19BE-D14B-8653-7707C3EF16C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{FC763E2B-1BB8-D248-8DD1-F66FE797A262}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" activeTab="1" xr2:uid="{FC763E2B-1BB8-D248-8DD1-F66FE797A262}"/>
   </bookViews>
   <sheets>
     <sheet name="Districts" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="131">
   <si>
     <t>County</t>
   </si>
@@ -398,12 +398,6 @@
   </si>
   <si>
     <t>Concord</t>
-  </si>
-  <si>
-    <t>04.26.2022</t>
-  </si>
-  <si>
-    <t>04.03.2015</t>
   </si>
   <si>
     <t>Rural Lands</t>
@@ -492,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -500,6 +494,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1146,7 +1141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4BA41B-4280-B747-9B6E-C79D73F6A3E5}">
   <dimension ref="A1:K144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B110" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1173,31 +1168,31 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>89</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>89</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>89</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>89</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>89</v>
@@ -1258,23 +1253,23 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -1990,7 +1985,7 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -4726,8 +4721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05389331-E65F-9747-B96F-F1FC2DF92AD8}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:T12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4822,35 +4817,35 @@
         <v>80</v>
       </c>
       <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" t="s">
         <v>122</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>123</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>124</v>
-      </c>
-      <c r="E12" t="s">
-        <v>125</v>
-      </c>
-      <c r="F12" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>102</v>
       </c>
-      <c r="B13" t="s">
-        <v>120</v>
+      <c r="B13" s="5">
+        <v>44677</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>103</v>
       </c>
-      <c r="B14" t="s">
-        <v>121</v>
+      <c r="B14" s="5">
+        <v>42097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>